<commit_message>
changing to online spreadhsheet
</commit_message>
<xml_diff>
--- a/data/worker_data.xlsx
+++ b/data/worker_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mess\CODE REPO\Producción PH - Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBC628B-A6A8-45A4-8627-32417E4382E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C540D9E2-9E8D-43F3-850B-EFA98A9021E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="67">
   <si>
     <t>FELIPE URDERO</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>Sexo</t>
+  </si>
+  <si>
+    <t>PRUEBA</t>
   </si>
 </sst>
 </file>
@@ -551,21 +554,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.6328125" customWidth="1"/>
+    <col min="2" max="3" width="22.6328125" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -582,7 +584,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -599,7 +601,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -616,7 +618,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -633,7 +635,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -650,7 +652,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -667,7 +669,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -684,7 +686,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -701,7 +703,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -718,7 +720,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -735,7 +737,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -752,7 +754,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -769,7 +771,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -786,7 +788,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -803,7 +805,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -820,7 +822,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -837,7 +839,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -854,7 +856,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -871,7 +873,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -888,7 +890,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -905,7 +907,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -922,7 +924,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -939,7 +941,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -956,7 +958,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -973,7 +975,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -990,7 +992,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1009,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1024,7 +1026,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1041,7 +1043,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1060,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1075,7 +1077,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1092,7 +1094,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1109,7 +1111,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1126,7 +1128,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1160,7 +1162,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1177,7 +1179,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +1196,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -1211,7 +1213,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1228,7 +1230,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1245,7 +1247,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1262,7 +1264,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1279,7 +1281,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1296,7 +1298,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1313,7 +1315,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1330,7 +1332,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -1347,7 +1349,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1364,7 +1366,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -1381,7 +1383,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1398,7 +1400,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -1415,7 +1417,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -1432,7 +1434,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -1447,6 +1449,40 @@
       </c>
       <c r="E52" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>51</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54">
+        <v>52</v>
+      </c>
+      <c r="D54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>